<commit_message>
use the project name
</commit_message>
<xml_diff>
--- a/project_data_wbs.xlsx
+++ b/project_data_wbs.xlsx
@@ -472,7 +472,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>project</t>
+          <t>SelfiePod</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -498,7 +498,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>project</t>
+          <t>SelfiePod</t>
         </is>
       </c>
     </row>
@@ -1673,7 +1673,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>project</t>
+          <t>SelfiePod</t>
         </is>
       </c>
     </row>
@@ -2148,7 +2148,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>project</t>
+          <t>SelfiePod</t>
         </is>
       </c>
     </row>
@@ -2598,7 +2598,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>project</t>
+          <t>SelfiePod</t>
         </is>
       </c>
     </row>
@@ -3023,7 +3023,7 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>project</t>
+          <t>SelfiePod</t>
         </is>
       </c>
     </row>

</xml_diff>